<commit_message>
I think BOM is complete
</commit_message>
<xml_diff>
--- a/Hardware/Basic/Bottom/NotSoSmartWatch-BASIC-BOTTOM-BOM.xlsx
+++ b/Hardware/Basic/Bottom/NotSoSmartWatch-BASIC-BOTTOM-BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Documents\Arduino\libraries\NotSoSmartWatch\Hardware\Basic\Bottom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdav2\Documents\EAGLE\NotSoSmartWatch\Hardware\Basic\Bottom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09586AC8-A7D7-48C7-853B-EFA2F477C8D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3E608B-DABC-4DC9-9761-4F573C4E418B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -626,7 +626,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -702,14 +702,6 @@
       <color theme="1"/>
       <name val="Segoe UI Historic"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -921,6 +913,15 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -930,16 +931,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="82">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1362,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" zoomScaleNormal="117" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1384,12 +1376,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -1402,14 +1394,14 @@
       </c>
       <c r="M1" s="6">
         <f>SUM(M5:M85)</f>
-        <v>83.733700000000013</v>
+        <v>20.039799999999996</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>23</v>
       </c>
       <c r="O1" s="6">
         <f>SUM(O5:O85)</f>
-        <v>5.5499999999999994E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
@@ -1461,24 +1453,24 @@
     </row>
     <row r="3" spans="1:16" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="16"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="18"/>
     </row>
     <row r="5" spans="1:16" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -1490,34 +1482,34 @@
       <c r="C5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="10" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="11">
         <v>1.26</v>
       </c>
       <c r="L5" s="2">
         <v>1</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="11">
         <f t="shared" ref="M5:M7" si="0">K5*L5</f>
         <v>1.26</v>
       </c>
@@ -1534,34 +1526,34 @@
       <c r="C6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="11">
         <v>0.59799999999999998</v>
       </c>
       <c r="L6" s="2">
         <v>1</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="11">
         <f t="shared" si="0"/>
         <v>0.59799999999999998</v>
       </c>
@@ -1578,36 +1570,36 @@
       <c r="C7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="11">
         <v>3.47</v>
       </c>
       <c r="L7" s="2">
-        <v>6</v>
-      </c>
-      <c r="M7" s="14">
+        <v>1</v>
+      </c>
+      <c r="M7" s="11">
         <f t="shared" si="0"/>
-        <v>20.82</v>
+        <v>3.47</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -1622,31 +1614,31 @@
       <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="11">
         <v>5.0599999999999996</v>
       </c>
       <c r="L8" s="2">
         <v>1</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="11">
         <f t="shared" ref="M8:M17" si="1">K8*L8</f>
         <v>5.0599999999999996</v>
       </c>
@@ -1663,36 +1655,36 @@
       <c r="C9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="11">
         <v>1.05</v>
       </c>
       <c r="L9" s="2">
-        <v>10</v>
-      </c>
-      <c r="M9" s="14">
+        <v>1</v>
+      </c>
+      <c r="M9" s="11">
         <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>1.05</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -1710,10 +1702,10 @@
       <c r="D10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -1722,21 +1714,21 @@
       <c r="H10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="11">
         <v>3.3099999999999997E-2</v>
       </c>
       <c r="L10" s="2">
-        <v>2</v>
-      </c>
-      <c r="M10" s="14">
+        <v>7</v>
+      </c>
+      <c r="M10" s="11">
         <f t="shared" si="1"/>
-        <v>6.6199999999999995E-2</v>
+        <v>0.23169999999999999</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -1751,42 +1743,40 @@
       <c r="C11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="11">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="L11" s="2">
-        <v>5</v>
-      </c>
-      <c r="M11" s="14">
+        <v>3</v>
+      </c>
+      <c r="M11" s="11">
         <f t="shared" si="1"/>
-        <v>2.9499999999999998E-2</v>
-      </c>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
+        <v>1.77E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="A12" s="14">
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1795,89 +1785,86 @@
       <c r="C12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="14">
+      <c r="K12" s="11">
         <v>0.1</v>
       </c>
       <c r="L12" s="2">
-        <v>3</v>
-      </c>
-      <c r="M12" s="14">
+        <v>1</v>
+      </c>
+      <c r="M12" s="11">
         <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="N12" s="14">
-        <v>1.8499999999999999E-2</v>
-      </c>
-      <c r="O12" s="14">
-        <f t="shared" ref="O12" si="2">L12*N12</f>
-        <v>5.5499999999999994E-2</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="14">
         <v>9</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="10" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="11">
         <v>3.11</v>
       </c>
       <c r="L13" s="2">
-        <v>5</v>
-      </c>
-      <c r="M13" s="14">
+        <v>1</v>
+      </c>
+      <c r="M13" s="11">
         <f t="shared" si="1"/>
-        <v>15.549999999999999</v>
+        <v>3.11</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="14">
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1886,45 +1873,43 @@
       <c r="C14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="10" t="s">
         <v>95</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="K14" s="14">
+      <c r="K14" s="11">
         <v>3.1600000000000003E-2</v>
       </c>
       <c r="L14" s="2">
-        <v>100</v>
-      </c>
-      <c r="M14" s="14">
+        <v>4</v>
+      </c>
+      <c r="M14" s="11">
         <f t="shared" si="1"/>
-        <v>3.16</v>
+        <v>0.12640000000000001</v>
       </c>
       <c r="N14" s="2"/>
-      <c r="O14" s="14">
-        <f t="shared" ref="O14" si="3">L14*N14</f>
-        <v>0</v>
-      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
+      <c r="A15" s="14">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1933,42 +1918,43 @@
       <c r="C15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="10" t="s">
         <v>98</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="J15" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="K15" s="14">
+      <c r="K15" s="11">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="L15" s="2">
-        <v>100</v>
-      </c>
-      <c r="M15" s="14">
+        <v>4</v>
+      </c>
+      <c r="M15" s="11">
         <f t="shared" si="1"/>
-        <v>0.59</v>
+        <v>2.3599999999999999E-2</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="18">
+      <c r="A16" s="14">
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1977,42 +1963,43 @@
       <c r="C16" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="10" t="s">
         <v>101</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="K16" s="14">
+      <c r="K16" s="11">
         <v>8.8999999999999999E-3</v>
       </c>
       <c r="L16" s="2">
-        <v>100</v>
-      </c>
-      <c r="M16" s="14">
+        <v>2</v>
+      </c>
+      <c r="M16" s="11">
         <f t="shared" si="1"/>
-        <v>0.89</v>
+        <v>1.78E-2</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:15" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="18">
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2021,42 +2008,43 @@
       <c r="C17" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="10" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="J17" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K17" s="11">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="L17" s="2">
-        <v>100</v>
-      </c>
-      <c r="M17" s="14">
+        <v>2</v>
+      </c>
+      <c r="M17" s="11">
         <f t="shared" si="1"/>
-        <v>0.59</v>
+        <v>1.18E-2</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="1:15" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -2065,45 +2053,43 @@
       <c r="C18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="K18" s="14">
+      <c r="K18" s="11">
         <v>6.7199999999999996E-2</v>
       </c>
       <c r="L18" s="2">
-        <v>100</v>
-      </c>
-      <c r="M18" s="14">
-        <f t="shared" ref="M18:M20" si="4">K18*L18</f>
-        <v>6.72</v>
+        <v>1</v>
+      </c>
+      <c r="M18" s="11">
+        <f t="shared" ref="M18:M20" si="2">K18*L18</f>
+        <v>6.7199999999999996E-2</v>
       </c>
       <c r="N18" s="2"/>
-      <c r="O18" s="14">
-        <f t="shared" ref="O18" si="5">L18*N18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2112,42 +2098,43 @@
       <c r="C19" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K19" s="11">
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="L19" s="2">
-        <v>100</v>
-      </c>
-      <c r="M19" s="14">
-        <f t="shared" si="4"/>
-        <v>1.5599999999999998</v>
+        <v>1</v>
+      </c>
+      <c r="M19" s="11">
+        <f t="shared" si="2"/>
+        <v>1.5599999999999999E-2</v>
       </c>
       <c r="N19" s="2"/>
-      <c r="O19" s="14"/>
-    </row>
-    <row r="20" spans="1:15" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -2156,78 +2143,80 @@
       <c r="C20" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="11">
         <v>0.44</v>
       </c>
       <c r="L20" s="2">
-        <v>6</v>
-      </c>
-      <c r="M20" s="14">
-        <f t="shared" si="4"/>
-        <v>2.64</v>
+        <v>5</v>
+      </c>
+      <c r="M20" s="11">
+        <f t="shared" si="2"/>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N20" s="2"/>
-      <c r="O20" s="14"/>
-    </row>
-    <row r="21" spans="1:15" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="14"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="11"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="14"/>
+      <c r="M21" s="11"/>
       <c r="N21" s="2"/>
-      <c r="O21" s="14"/>
-    </row>
-    <row r="22" spans="1:15" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15" t="s">
+      <c r="O21" s="11"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-    </row>
-    <row r="23" spans="1:15" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A23" s="18">
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+    </row>
+    <row r="23" spans="1:16" s="2" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -2236,43 +2225,43 @@
       <c r="C23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I23" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="K23" s="14">
+      <c r="K23" s="11">
         <v>2.68</v>
       </c>
       <c r="L23" s="2">
-        <v>5</v>
-      </c>
-      <c r="M23" s="14">
+        <v>1</v>
+      </c>
+      <c r="M23" s="11">
         <f>K23*L23</f>
-        <v>13.4</v>
-      </c>
-      <c r="O23" s="14">
-        <f t="shared" ref="O22:O23" si="6">L23*N23</f>
+        <v>2.68</v>
+      </c>
+      <c r="O23" s="11">
+        <f t="shared" ref="O23" si="3">L23*N23</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="11.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2288,28 +2277,30 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
-    </row>
-    <row r="25" spans="1:15" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15" t="s">
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-    </row>
-    <row r="26" spans="1:15" ht="11.4" x14ac:dyDescent="0.25">
-      <c r="A26" s="18">
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
         <f>1</f>
         <v>1</v>
       </c>
@@ -2326,14 +2317,15 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="14"/>
+      <c r="K26" s="11"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="14">
+      <c r="M26" s="11">
         <f>K26*L26</f>
         <v>0</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>